<commit_message>
correcciones vacio y ok
</commit_message>
<xml_diff>
--- a/Ejemplo Laptops.xlsx
+++ b/Ejemplo Laptops.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\go\src\ControlInvetario\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE5FD52E-F4F5-4654-9B00-8F2F4C8C3167}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE4003C-2818-43C1-B145-4B5033A34392}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{0ACF1C88-95D9-447B-9F42-52A8AD798E73}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="56">
   <si>
     <t>fecha</t>
   </si>
@@ -63,9 +63,6 @@
     <t>DISCO</t>
   </si>
   <si>
-    <t xml:space="preserve"> SERIE disco</t>
-  </si>
-  <si>
     <t>SERIE ORIGINAL</t>
   </si>
   <si>
@@ -190,6 +187,12 @@
   </si>
   <si>
     <t>1s2466D79R9TW53Y</t>
+  </si>
+  <si>
+    <t>Probando</t>
+  </si>
+  <si>
+    <t>SERIE disco</t>
   </si>
 </sst>
 </file>
@@ -728,7 +731,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,38 +779,38 @@
         <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="Q1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="7"/>
       <c r="C2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="G2" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="G2" s="16" t="s">
-        <v>21</v>
       </c>
       <c r="H2" s="16">
         <v>4</v>
@@ -820,39 +823,41 @@
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="N2" s="16" t="s">
         <v>23</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>24</v>
       </c>
       <c r="O2" s="16">
         <v>14</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
       <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="16" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" s="16" t="s">
-        <v>21</v>
       </c>
       <c r="H3" s="16">
         <v>4</v>
@@ -865,39 +870,41 @@
       </c>
       <c r="K3" s="17"/>
       <c r="L3" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="16" t="s">
         <v>26</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>27</v>
       </c>
       <c r="O3" s="16">
         <v>14</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="Q3" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="7"/>
       <c r="C4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="F4" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H4" s="16">
         <v>5</v>
@@ -910,64 +917,66 @@
       </c>
       <c r="K4" s="16"/>
       <c r="L4" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M4" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="16" t="s">
         <v>29</v>
-      </c>
-      <c r="N4" s="16" t="s">
-        <v>30</v>
       </c>
       <c r="O4" s="16">
         <v>14</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="Q4" s="9" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="7"/>
       <c r="C5" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E5" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="H5" s="12">
         <v>3</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J5" s="11">
         <v>4</v>
       </c>
       <c r="K5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O5" s="12">
         <v>14</v>
       </c>
       <c r="P5" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q5" s="9"/>
     </row>
@@ -975,44 +984,44 @@
       <c r="A6" s="6"/>
       <c r="B6" s="7"/>
       <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="G6" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="H6" s="11">
         <v>3</v>
       </c>
       <c r="I6" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J6" s="11">
         <v>4</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="L6" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M6" s="11"/>
       <c r="N6" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O6" s="12">
         <v>14</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q6" s="9"/>
     </row>
@@ -1020,44 +1029,44 @@
       <c r="A7" s="6"/>
       <c r="B7" s="7"/>
       <c r="C7" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E7" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="H7" s="11">
         <v>3</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J7" s="11">
         <v>4</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L7" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M7" s="11"/>
       <c r="N7" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O7" s="12">
         <v>14</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q7" s="9"/>
     </row>
@@ -1065,44 +1074,44 @@
       <c r="A8" s="6"/>
       <c r="B8" s="7"/>
       <c r="C8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>32</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>33</v>
       </c>
       <c r="H8" s="11">
         <v>3</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J8" s="11">
         <v>4</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L8" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M8" s="11"/>
       <c r="N8" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="O8" s="12">
         <v>14</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q8" s="9"/>
     </row>
@@ -1110,44 +1119,44 @@
       <c r="A9" s="6"/>
       <c r="B9" s="7"/>
       <c r="C9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E9" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>44</v>
-      </c>
-      <c r="G9" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="H9" s="11">
         <v>2</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="11">
         <v>4</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L9" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O9" s="14">
         <v>14</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q9" s="9"/>
     </row>
@@ -1155,44 +1164,44 @@
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H10" s="14">
         <v>3</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J10" s="11">
         <v>4</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L10" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O10" s="14">
         <v>14</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q10" s="9"/>
     </row>
@@ -1200,44 +1209,44 @@
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="E11" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H11" s="14">
         <v>3</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J11" s="11">
         <v>4</v>
       </c>
       <c r="K11" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O11" s="14">
         <v>14</v>
       </c>
       <c r="P11" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q11" s="9"/>
     </row>

</xml_diff>